<commit_message>
Added PIL image editing, Verifying existing functions
</commit_message>
<xml_diff>
--- a/coord.xlsx
+++ b/coord.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen.lang\Desktop\CAB\6 - HMC Data Processing\07-Visualization\Fun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\InjuryVisualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBC4F89-2F25-44B6-8F5D-24115F4CFE72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="5115"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Circle" sheetId="1" r:id="rId1"/>
@@ -103,9 +104,6 @@
     <t>xSh</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>ySh</t>
   </si>
   <si>
@@ -197,12 +195,15 @@
   </si>
   <si>
     <t>Femur Lateral Left</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1009,10 +1010,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1135,7 +1136,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1">
         <v>280</v>
@@ -1149,7 +1150,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1">
         <v>518</v>
@@ -1219,7 +1220,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1">
         <v>340</v>
@@ -1233,7 +1234,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1">
         <v>460</v>
@@ -1275,7 +1276,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1">
         <v>366</v>
@@ -1289,7 +1290,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1">
         <v>334</v>
@@ -1303,7 +1304,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1">
         <v>312</v>
@@ -1317,7 +1318,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1">
         <v>301</v>
@@ -1331,7 +1332,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1">
         <v>299</v>
@@ -1345,7 +1346,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1">
         <v>300</v>
@@ -1359,7 +1360,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1">
         <v>301</v>
@@ -1373,7 +1374,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1">
         <v>305</v>
@@ -1387,7 +1388,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1">
         <v>310</v>
@@ -1401,7 +1402,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="1">
         <v>319</v>
@@ -1415,7 +1416,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1">
         <v>434</v>
@@ -1429,7 +1430,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
         <v>465</v>
@@ -1443,7 +1444,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1">
         <v>490</v>
@@ -1457,7 +1458,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1">
         <v>501</v>
@@ -1471,7 +1472,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1">
         <v>500</v>
@@ -1485,7 +1486,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1">
         <v>499</v>
@@ -1499,7 +1500,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1">
         <v>496</v>
@@ -1513,7 +1514,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1">
         <v>493</v>
@@ -1527,7 +1528,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1">
         <v>491</v>
@@ -1541,7 +1542,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1">
         <v>486</v>
@@ -1560,11 +1561,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,18 +1585,18 @@
         <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1">
         <v>25</v>
@@ -1615,7 +1616,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1">
         <v>25</v>
@@ -1635,7 +1636,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>15</v>
@@ -1815,7 +1816,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1">
         <v>35</v>
@@ -1835,7 +1836,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1">
         <v>35</v>

</xml_diff>

<commit_message>
separated head metrics (BrIC and HIC36), extra documentation, ran on 2020 results
</commit_message>
<xml_diff>
--- a/coord.xlsx
+++ b/coord.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\InjuryVisualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\InjuryVisualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBC4F89-2F25-44B6-8F5D-24115F4CFE72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3FBE01-8992-4256-BDA3-3FEA22C0C2C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>X</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Midfoot Right</t>
   </si>
   <si>
-    <t>Head</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -198,6 +195,12 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Head BrIC</t>
+  </si>
+  <si>
+    <t>Head HIC</t>
   </si>
 </sst>
 </file>
@@ -1014,12 +1017,12 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,16 +1041,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1">
         <v>400</v>
       </c>
       <c r="C2" s="1">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1">
-        <v>22.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1058,10 +1061,10 @@
         <v>400</v>
       </c>
       <c r="C3" s="1">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D3" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1136,7 +1139,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1">
         <v>280</v>
@@ -1150,7 +1153,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1">
         <v>518</v>
@@ -1192,7 +1195,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>324</v>
@@ -1206,7 +1209,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>474</v>
@@ -1220,7 +1223,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1">
         <v>340</v>
@@ -1234,7 +1237,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1">
         <v>460</v>
@@ -1276,7 +1279,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1">
         <v>366</v>
@@ -1290,7 +1293,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1">
         <v>334</v>
@@ -1304,7 +1307,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1">
         <v>312</v>
@@ -1318,7 +1321,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1">
         <v>301</v>
@@ -1332,7 +1335,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1">
         <v>299</v>
@@ -1346,7 +1349,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1">
         <v>300</v>
@@ -1360,7 +1363,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1">
         <v>301</v>
@@ -1374,7 +1377,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1">
         <v>305</v>
@@ -1388,7 +1391,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1">
         <v>310</v>
@@ -1402,7 +1405,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1">
         <v>319</v>
@@ -1416,7 +1419,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1">
         <v>434</v>
@@ -1430,7 +1433,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1">
         <v>465</v>
@@ -1444,7 +1447,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1">
         <v>490</v>
@@ -1458,7 +1461,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1">
         <v>501</v>
@@ -1472,7 +1475,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1">
         <v>500</v>
@@ -1486,7 +1489,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1">
         <v>499</v>
@@ -1500,7 +1503,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1">
         <v>496</v>
@@ -1514,7 +1517,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1">
         <v>493</v>
@@ -1528,7 +1531,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1">
         <v>491</v>
@@ -1542,7 +1545,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1">
         <v>486</v>
@@ -1562,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,27 +1582,27 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B2" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1">
         <v>400</v>
@@ -1608,7 +1611,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1616,19 +1619,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1">
         <v>400</v>
       </c>
       <c r="D3" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -1639,16 +1642,16 @@
         <v>30</v>
       </c>
       <c r="B4" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
         <v>400</v>
       </c>
       <c r="D4" s="1">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1656,19 +1659,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="D5" s="1">
-        <v>7.5</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1">
-        <v>270</v>
+        <v>125</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1682,7 +1685,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="1">
-        <v>476</v>
+        <v>320</v>
       </c>
       <c r="D6" s="1">
         <v>7.5</v>
@@ -1696,22 +1699,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1">
-        <v>228</v>
+        <v>476</v>
       </c>
       <c r="D7" s="1">
-        <v>12.5</v>
+        <v>7.5</v>
       </c>
       <c r="E7" s="1">
-        <v>400</v>
+        <v>270</v>
       </c>
       <c r="F7" s="1">
-        <v>-85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,7 +1725,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="1">
-        <v>572</v>
+        <v>228</v>
       </c>
       <c r="D8" s="1">
         <v>12.5</v>
@@ -1731,27 +1734,27 @@
         <v>400</v>
       </c>
       <c r="F8" s="1">
-        <v>85</v>
+        <v>-85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
         <v>35</v>
       </c>
       <c r="C9" s="1">
-        <v>204</v>
+        <v>572</v>
       </c>
       <c r="D9" s="1">
         <v>12.5</v>
       </c>
       <c r="E9" s="1">
-        <v>595</v>
+        <v>400</v>
       </c>
       <c r="F9" s="1">
-        <v>-86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1762,7 +1765,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="1">
-        <v>592</v>
+        <v>204</v>
       </c>
       <c r="D10" s="1">
         <v>12.5</v>
@@ -1771,27 +1774,27 @@
         <v>595</v>
       </c>
       <c r="F10" s="1">
-        <v>86</v>
+        <v>-86</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1">
-        <v>313</v>
+        <v>592</v>
       </c>
       <c r="D11" s="1">
         <v>12.5</v>
       </c>
       <c r="E11" s="1">
-        <v>848</v>
+        <v>595</v>
       </c>
       <c r="F11" s="1">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1802,7 +1805,7 @@
         <v>40</v>
       </c>
       <c r="C12" s="1">
-        <v>483</v>
+        <v>313</v>
       </c>
       <c r="D12" s="1">
         <v>12.5</v>
@@ -1811,27 +1814,27 @@
         <v>848</v>
       </c>
       <c r="F12" s="1">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1">
-        <v>335</v>
+        <v>483</v>
       </c>
       <c r="D13" s="1">
         <v>12.5</v>
       </c>
       <c r="E13" s="1">
-        <v>1192</v>
+        <v>848</v>
       </c>
       <c r="F13" s="1">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1842,7 +1845,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="1">
-        <v>467</v>
+        <v>335</v>
       </c>
       <c r="D14" s="1">
         <v>12.5</v>
@@ -1851,6 +1854,26 @@
         <v>1192</v>
       </c>
       <c r="F14" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1">
+        <v>467</v>
+      </c>
+      <c r="D15" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1192</v>
+      </c>
+      <c r="F15" s="1">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified head object shape, re-ran on all
</commit_message>
<xml_diff>
--- a/coord.xlsx
+++ b/coord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\InjuryVisualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3FBE01-8992-4256-BDA3-3FEA22C0C2C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D9736B-1DA7-4150-BD6D-968B8A3154A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1568,7 +1568,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,7 +1602,7 @@
         <v>59</v>
       </c>
       <c r="B2" s="1">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1">
         <v>400</v>

</xml_diff>

<commit_message>
Bug fix, nasal and maxilla out of order
</commit_message>
<xml_diff>
--- a/coord.xlsx
+++ b/coord.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\InjuryVisualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D9736B-1DA7-4150-BD6D-968B8A3154A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE30E1C8-2A6F-4B0E-82DE-82A5C256AD2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1568,7 +1568,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>30</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>

</xml_diff>